<commit_message>
Updates on BOM, and shit on the design
Added order locations and discovered that mouser and digikey are out of
atmega32u4s. Straight up fuck! They don't get any for months. Last
minute redesign? Pay a shit ton more and get them from
sparkfun/adafruit, or are they out too?! Maybe this is a world wide
shortage. People can't get their hands on built in usb support and
engineers all over fucking everywhere are killing each other to get
their oily hands all over these sleek, sexy chips. I would kill a man to
hold one right now, and then another man to keep it forever. Okay,
bedtime.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\GitHub\Tesa\BOM\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
   <si>
     <t>Refdes</t>
   </si>
@@ -87,9 +92,6 @@
     <t>U101</t>
   </si>
   <si>
-    <t>AtMega32U4</t>
-  </si>
-  <si>
     <t>CSTCE8M00G55-R0</t>
   </si>
   <si>
@@ -193,6 +195,33 @@
   </si>
   <si>
     <t>16pin hdr total</t>
+  </si>
+  <si>
+    <t>Price per unit (for 10)</t>
+  </si>
+  <si>
+    <t>Order from</t>
+  </si>
+  <si>
+    <t>AtMega32U4RC-AU</t>
+  </si>
+  <si>
+    <t>Literal fuck!!!</t>
+  </si>
+  <si>
+    <t>Can't buy!!!</t>
+  </si>
+  <si>
+    <t>M (71-CRCW0603-4.7K-E3)</t>
+  </si>
+  <si>
+    <t>M (71-CRCW0603-1.43K-E3)</t>
+  </si>
+  <si>
+    <t>M (71-CRCW0603-22-E3)</t>
+  </si>
+  <si>
+    <t>M (652-MF-MSMF050-2)</t>
   </si>
 </sst>
 </file>
@@ -270,11 +299,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -282,8 +308,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -296,6 +328,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -344,7 +379,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,7 +414,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,92 +623,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
-    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -681,51 +732,57 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>45</v>
-      </c>
       <c r="G4" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
+      <c r="J4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>45</v>
-      </c>
       <c r="G5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" t="s">
         <v>55</v>
       </c>
-      <c r="H5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -733,67 +790,81 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
         <v>35</v>
       </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>45</v>
-      </c>
       <c r="G6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
-        <v>25</v>
+      <c r="C7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="6">
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
-      </c>
-      <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="H7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>22</v>
       </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" t="s">
+        <v>43</v>
+      </c>
+      <c r="H8" t="s">
         <v>44</v>
       </c>
-      <c r="F8" t="s">
-        <v>45</v>
-      </c>
-      <c r="G8" t="s">
-        <v>37</v>
-      </c>
-      <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>36</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -801,170 +872,178 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>66</v>
+      </c>
+      <c r="D9">
+        <v>0.20100000000000001</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
         <v>16</v>
       </c>
-      <c r="G9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="E10" t="s">
-        <v>25</v>
+        <v>28</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="G10" t="s">
-        <v>57</v>
-      </c>
-      <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="5"/>
       <c r="E11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>24</v>
       </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14" s="5"/>
-      <c r="E14" t="s">
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="5"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" t="s">
-        <v>49</v>
-      </c>
-      <c r="F16" s="5"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>27</v>
       </c>
-      <c r="E17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="5"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="D10:D14"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="H6:H10"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="H13:H17"/>
+    <mergeCell ref="J6:J10"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added circle outline in correct layers
To power board
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erik\Documents\GitHub\Tesa\BOM\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
   <si>
     <t>Refdes</t>
   </si>
@@ -92,6 +87,9 @@
     <t>U101</t>
   </si>
   <si>
+    <t>AtMega32U4</t>
+  </si>
+  <si>
     <t>CSTCE8M00G55-R0</t>
   </si>
   <si>
@@ -195,33 +193,6 @@
   </si>
   <si>
     <t>16pin hdr total</t>
-  </si>
-  <si>
-    <t>Price per unit (for 10)</t>
-  </si>
-  <si>
-    <t>Order from</t>
-  </si>
-  <si>
-    <t>AtMega32U4RC-AU</t>
-  </si>
-  <si>
-    <t>Literal fuck!!!</t>
-  </si>
-  <si>
-    <t>Can't buy!!!</t>
-  </si>
-  <si>
-    <t>M (71-CRCW0603-4.7K-E3)</t>
-  </si>
-  <si>
-    <t>M (71-CRCW0603-1.43K-E3)</t>
-  </si>
-  <si>
-    <t>M (71-CRCW0603-22-E3)</t>
-  </si>
-  <si>
-    <t>M (652-MF-MSMF050-2)</t>
   </si>
 </sst>
 </file>
@@ -299,8 +270,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -308,14 +282,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -328,9 +296,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -379,7 +344,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,7 +379,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -623,108 +588,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
-    <col min="8" max="8" width="20.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.140625" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4" t="s">
+      <c r="D1" s="1"/>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -732,57 +681,51 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4">
-        <v>1.4999999999999999E-2</v>
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="G4" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" t="s">
-        <v>53</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
+        <v>55</v>
       </c>
       <c r="H5" t="s">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -790,81 +733,67 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6">
-        <v>1.4999999999999999E-2</v>
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
+        <v>36</v>
       </c>
       <c r="E6" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
-      </c>
-      <c r="H6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <v>22</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1.4999999999999999E-2</v>
+      <c r="C7" t="s">
+        <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
       </c>
       <c r="G7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="3">
         <v>22</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
       <c r="E8" t="s">
-        <v>25</v>
+        <v>44</v>
+      </c>
+      <c r="F8" t="s">
+        <v>45</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
-      </c>
-      <c r="H8" t="s">
-        <v>44</v>
-      </c>
-      <c r="I8" t="s">
-        <v>36</v>
-      </c>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -872,178 +801,170 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9">
-        <v>0.20100000000000001</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
       </c>
       <c r="G9" t="s">
-        <v>45</v>
-      </c>
-      <c r="H9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" t="s">
-        <v>48</v>
-      </c>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>51</v>
+        <v>25</v>
       </c>
       <c r="G10" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" t="s">
-        <v>56</v>
-      </c>
-      <c r="J10" s="5"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="5"/>
       <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
       </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="5"/>
       <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5"/>
       <c r="E13" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="5"/>
       <c r="E14" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="F14" s="5"/>
-      <c r="G14" t="s">
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="H14" s="5"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G15" t="s">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>28</v>
       </c>
-      <c r="H15" s="5"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" t="s">
-        <v>48</v>
-      </c>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="G17" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="5"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="F10:F14"/>
-    <mergeCell ref="H13:H17"/>
-    <mergeCell ref="J6:J10"/>
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="D10:D14"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="H6:H10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Added the TLC59711 everywhere!!
We missed it. We should all feel somewhat ashamed to have missed such an
obvious omission. Some minor changes to inventory list as well.
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t>Refdes</t>
   </si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>16pin hdr total</t>
+  </si>
+  <si>
+    <t>U102</t>
+  </si>
+  <si>
+    <t>TLC59711</t>
   </si>
 </sst>
 </file>
@@ -272,15 +278,15 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -588,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,46 +613,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -755,7 +761,7 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>22</v>
       </c>
       <c r="C7" t="s">
@@ -776,7 +782,7 @@
       <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>22</v>
       </c>
       <c r="C8" t="s">
@@ -887,7 +893,7 @@
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C14" t="s">
@@ -954,6 +960,14 @@
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>